<commit_message>
add specific factor mode
</commit_message>
<xml_diff>
--- a/examples/exporter/tables/factor_table.xlsx
+++ b/examples/exporter/tables/factor_table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\go\src\github.com\nekohor\other\app\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\go\src\github.com\nekohor\gomon\examples\exporter\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7242" yWindow="0" windowWidth="18318" windowHeight="7782"/>
+    <workbookView xWindow="8266" yWindow="0" windowWidth="18318" windowHeight="7782"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,103 +62,103 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>sym_flt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leveling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asym_flt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shape_series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cast_fm_stand_series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fm_center_ofs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>r2_center_ofs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calc_length_series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clg_calc_length</t>
+  </si>
+  <si>
+    <t>mfg_calc_length</t>
+  </si>
+  <si>
+    <t>calc_length1</t>
+  </si>
+  <si>
+    <t>calc_length2</t>
+  </si>
+  <si>
+    <t>calc_length3</t>
+  </si>
+  <si>
+    <t>calc_length4</t>
+  </si>
+  <si>
+    <t>calc_length5</t>
+  </si>
+  <si>
+    <t>calc_length6</t>
+  </si>
+  <si>
+    <t>calc_length7</t>
+  </si>
+  <si>
+    <t>fm_calc_length</t>
+  </si>
+  <si>
+    <t>flt_calc_length</t>
+  </si>
+  <si>
+    <t>r2dt_calc_length</t>
+  </si>
+  <si>
+    <t>r2dw_calc_length</t>
+  </si>
+  <si>
+    <t>ct_calc_length</t>
+  </si>
+  <si>
+    <t>fet_calc_length</t>
+  </si>
+  <si>
+    <t>fdt_calc_length</t>
+  </si>
+  <si>
+    <t>looper_angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>diff_rolling_force</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature_series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>crown40</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>wedge40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sym_flt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>leveling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>asym_flt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shape_series</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cast_fm_stand_series</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fm_center_ofs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>r2_center_ofs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>calc_length_series</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>clg_calc_length</t>
-  </si>
-  <si>
-    <t>mfg_calc_length</t>
-  </si>
-  <si>
-    <t>calc_length1</t>
-  </si>
-  <si>
-    <t>calc_length2</t>
-  </si>
-  <si>
-    <t>calc_length3</t>
-  </si>
-  <si>
-    <t>calc_length4</t>
-  </si>
-  <si>
-    <t>calc_length5</t>
-  </si>
-  <si>
-    <t>calc_length6</t>
-  </si>
-  <si>
-    <t>calc_length7</t>
-  </si>
-  <si>
-    <t>fm_calc_length</t>
-  </si>
-  <si>
-    <t>flt_calc_length</t>
-  </si>
-  <si>
-    <t>r2dt_calc_length</t>
-  </si>
-  <si>
-    <t>r2dw_calc_length</t>
-  </si>
-  <si>
-    <t>ct_calc_length</t>
-  </si>
-  <si>
-    <t>fet_calc_length</t>
-  </si>
-  <si>
-    <t>fdt_calc_length</t>
-  </si>
-  <si>
-    <t>looper_angle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>diff_rolling_force</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>temperature_series</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -515,7 +515,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.15"/>
@@ -528,21 +528,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -551,21 +551,21 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -576,10 +576,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -590,10 +590,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -604,74 +604,74 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>